<commit_message>
Upgrade cypress to 10.7 for testing quickview iframe case, recoding and fixed element to testing in the new website  (.pl)
</commit_message>
<xml_diff>
--- a/cypress/fixtures/goldenData/produce_detail_db.xlsx
+++ b/cypress/fixtures/goldenData/produce_detail_db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\awika-portfolio\automationpractice\cypress\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\awika-portfolio\automationpractice\cypress\fixtures\goldenData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69523B54-417E-4094-939B-5737E22BD14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2786525B-FF05-46DE-86AF-1073979C10E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7515" yWindow="-12855" windowWidth="17625" windowHeight="10395" xr2:uid="{78432280-16EC-44C7-9ABF-02394648B95C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{78432280-16EC-44C7-9ABF-02394648B95C}"/>
   </bookViews>
   <sheets>
     <sheet name="product" sheetId="1" r:id="rId1"/>
@@ -693,10 +693,10 @@
   <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -789,7 +789,7 @@
       <c r="F2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="13">
         <v>16.510000000000002</v>
       </c>
       <c r="H2" s="14" t="s">
@@ -841,7 +841,7 @@
       <c r="F3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="11">
         <v>27</v>
       </c>
       <c r="H3" s="15" t="s">
@@ -891,7 +891,7 @@
       <c r="F4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="11">
         <v>26</v>
       </c>
       <c r="H4" s="15" t="s">
@@ -941,8 +941,8 @@
       <c r="F5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="9">
-        <v>50.99</v>
+      <c r="G5" s="11">
+        <v>51</v>
       </c>
       <c r="H5" s="15" t="s">
         <v>65</v>
@@ -991,13 +991,13 @@
       <c r="F6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="11">
         <v>30.51</v>
       </c>
       <c r="H6" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="11">
         <v>28.98</v>
       </c>
       <c r="J6" s="11">
@@ -1047,12 +1047,13 @@
       <c r="F7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="11">
         <v>30.5</v>
       </c>
       <c r="H7" s="15" t="s">
         <v>65</v>
       </c>
+      <c r="I7" s="11"/>
       <c r="K7" s="1" t="s">
         <v>46</v>
       </c>
@@ -1097,13 +1098,13 @@
       <c r="F8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="11">
         <v>20.5</v>
       </c>
       <c r="H8" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="11">
         <v>16.399999999999999</v>
       </c>
       <c r="J8" s="11">

</xml_diff>